<commit_message>
1st commit on 3rd July 2021
</commit_message>
<xml_diff>
--- a/main/.data/byPair/momentum/[2017][HuyNguyen]-TradingView.xlsx
+++ b/main/.data/byPair/momentum/[2017][HuyNguyen]-TradingView.xlsx
@@ -7,14 +7,15 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="USDBTC" sheetId="1" r:id="rId1"/>
+    <sheet name="PAIR2" sheetId="1" r:id="rId1"/>
+    <sheet name="VNDUSD" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
   <si>
     <t>MONTH</t>
   </si>
@@ -28,12 +29,12 @@
     <t>POSITION</t>
   </si>
   <si>
+    <t>15MIN CHART</t>
+  </si>
+  <si>
     <t>1HR CHART</t>
   </si>
   <si>
-    <t>15MIN CHART</t>
-  </si>
-  <si>
     <t>PROFIT R</t>
   </si>
   <si>
@@ -46,19 +47,25 @@
     <t>SUM</t>
   </si>
   <si>
-    <t>21:36:29.571526</t>
-  </si>
-  <si>
-    <t>buy</t>
-  </si>
-  <si>
-    <t>LINK 1 HOUR</t>
-  </si>
-  <si>
-    <t>LINK 15-MIN</t>
-  </si>
-  <si>
-    <t>my comment</t>
+    <t>14:58:01.136710</t>
+  </si>
+  <si>
+    <t>Sell</t>
+  </si>
+  <si>
+    <t>link 1</t>
+  </si>
+  <si>
+    <t>link 2</t>
+  </si>
+  <si>
+    <t>this is my comment</t>
+  </si>
+  <si>
+    <t>14:57:30.000793</t>
+  </si>
+  <si>
+    <t>14:57:03.901108</t>
   </si>
 </sst>
 </file>
@@ -452,10 +459,10 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
@@ -470,16 +477,129 @@
         <v>13</v>
       </c>
       <c r="G2" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I2" s="1">
+        <v>810</v>
+      </c>
+      <c r="J2" s="1">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="5" max="6" width="35.7109375" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1">
+        <v>3</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="1">
+        <v>610</v>
+      </c>
       <c r="J2" s="1">
-        <v>5</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1">
+        <v>3</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="1">
+        <v>410</v>
+      </c>
+      <c r="J3" s="1">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>